<commit_message>
Tested code - altered then reverted excel
</commit_message>
<xml_diff>
--- a/documents/košarka_evidencija.xlsx
+++ b/documents/košarka_evidencija.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding projects\KosarkaManager\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ACD2A5-EEB5-42A6-823E-212BF0F7A860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81591AE4-D5A7-4095-BF46-646DA19734D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,7 +642,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I31" sqref="I3:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>